<commit_message>
Started wallpaper selection implementation
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\422Group4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>Door closed</t>
   </si>
@@ -150,9 +155,6 @@
     <t>http://www.flaticon.com/free-icon/key-hole_16526</t>
   </si>
   <si>
-    <t>http://www.flaticon.com/free-icon/speech-message_14578</t>
-  </si>
-  <si>
     <t>Abstract</t>
   </si>
   <si>
@@ -310,6 +312,21 @@
   </si>
   <si>
     <t>http://www.orangefreesounds.com/jetsons-doorbell/</t>
+  </si>
+  <si>
+    <t>http://www.flaticon.com/free-icon/note-black-paper-with-text-lines_34074</t>
+  </si>
+  <si>
+    <t>Landscapes</t>
+  </si>
+  <si>
+    <t>http://www.flaticon.com/free-icon/landscape_92744</t>
+  </si>
+  <si>
+    <t>Holidays</t>
+  </si>
+  <si>
+    <t>http://www.flaticon.com/free-icon/fireworks_108980</t>
   </si>
 </sst>
 </file>
@@ -620,7 +637,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +686,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -813,90 +830,106 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
         <v>75</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
         <v>77</v>
-      </c>
-      <c r="B23" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
         <v>79</v>
-      </c>
-      <c r="B24" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
         <v>81</v>
-      </c>
-      <c r="B25" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" t="s">
         <v>85</v>
       </c>
-      <c r="B27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
         <v>94</v>
-      </c>
-      <c r="B32" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -917,26 +950,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -956,98 +989,98 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1067,10 +1100,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
         <v>73</v>
-      </c>
-      <c r="B1" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented setting of date/time formats
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Main Icons" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="118">
   <si>
     <t>Door closed</t>
   </si>
@@ -363,6 +363,24 @@
   </si>
   <si>
     <t>https://wallpaperscraft.com/wallpaper/halloween_holiday_pumpkin_background_62754</t>
+  </si>
+  <si>
+    <t>Textures</t>
+  </si>
+  <si>
+    <t>http://www.flaticon.com/free-icon/bricks_104031</t>
+  </si>
+  <si>
+    <t>http://www.flaticon.com/free-icon/left-arrow-key_60965</t>
+  </si>
+  <si>
+    <t>http://www.flaticon.com/free-icon/keyboard-right-arrow-button_60758</t>
+  </si>
+  <si>
+    <t>Arrow left</t>
+  </si>
+  <si>
+    <t>Arrow right</t>
   </si>
 </sst>
 </file>
@@ -398,9 +416,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,290 +707,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A20" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B29" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>98</v>
-      </c>
-      <c r="B29" t="s">
-        <v>99</v>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -976,83 +1003,110 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B10" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B11" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B13" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="14" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="15" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B15" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1066,104 +1120,107 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1176,17 +1233,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented doorbell chime selection and began video capability
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\422Group4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main Icons" sheetId="1" r:id="rId1"/>
-    <sheet name="Wallpapers" sheetId="2" r:id="rId2"/>
-    <sheet name="Weather" sheetId="3" r:id="rId3"/>
-    <sheet name="Sounds" sheetId="4" r:id="rId4"/>
+    <sheet name="Videos" sheetId="5" r:id="rId2"/>
+    <sheet name="Wallpapers" sheetId="2" r:id="rId3"/>
+    <sheet name="Weather" sheetId="3" r:id="rId4"/>
+    <sheet name="Sounds" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>Door closed</t>
   </si>
@@ -60,9 +66,6 @@
     <t>House alarm</t>
   </si>
   <si>
-    <t>http://robotmonkeys.net/wp-content/uploads/softrains-twitter_files/home-security.png</t>
-  </si>
-  <si>
     <t>Emergency</t>
   </si>
   <si>
@@ -361,6 +364,36 @@
   </si>
   <si>
     <t>Language Flags</t>
+  </si>
+  <si>
+    <t>Grandma</t>
+  </si>
+  <si>
+    <t>http://www.shutterstock.com/video/clip-7209262-stock-footage-silly-grandma-making-funny-faces-at-the-camera.html</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>http://www.flaticon.com/free-icon/photo-camera_3901</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>http://www.flaticon.com/free-icon/chat-bubbles-with-ellipsis_61516</t>
+  </si>
+  <si>
+    <t>Cool Guy</t>
+  </si>
+  <si>
+    <t>https://www.shutterstock.com/video/clip-11529716-stock-footage-handsome-man-in-a-light-blue-jacket-standing-outside-on-a-sunny-summer-day-with-a-green-background.html</t>
+  </si>
+  <si>
+    <t>Couple</t>
+  </si>
+  <si>
+    <t>http://www.shutterstock.com/video/clip-5574770-stock-footage-young-happy-couple-standing-on-house-porch.html</t>
   </si>
 </sst>
 </file>
@@ -679,7 +712,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -687,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,7 +733,7 @@
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -708,7 +741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -716,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -724,26 +757,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -751,196 +781,212 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -950,6 +996,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -964,74 +1049,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1039,7 +1124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -1054,98 +1139,98 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1153,7 +1238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1170,42 +1255,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced 'fireworks' wallpaper with 'birthday'
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Main Icons" sheetId="1" r:id="rId1"/>
@@ -348,12 +348,6 @@
     <t>https://wallpaperscraft.com/wallpaper/wreath_new_year_spruce_snow_winter_98974</t>
   </si>
   <si>
-    <t>fireworks</t>
-  </si>
-  <si>
-    <t>https://wallpaperscraft.com/wallpaper/sydney_fireworks_holiday_joy_872</t>
-  </si>
-  <si>
     <t>Halloween</t>
   </si>
   <si>
@@ -394,6 +388,12 @@
   </si>
   <si>
     <t>http://www.shutterstock.com/video/clip-5574770-stock-footage-young-happy-couple-standing-on-house-porch.html</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>https://wallpaperscraft.com/download/pie_candles_birthday_1371/1080x1920</t>
   </si>
 </sst>
 </file>
@@ -967,26 +967,26 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -999,7 +999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1007,26 +1007,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1038,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,18 +1097,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished camera/doorbell (I hope?)
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Main Icons" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>Door closed</t>
   </si>
@@ -396,16 +396,22 @@
     <t>https://wallpaperscraft.com/download/pie_candles_birthday_1371/1080x1920</t>
   </si>
   <si>
-    <t>http://www.flaticon.com/free-icon/mask_108961</t>
-  </si>
-  <si>
-    <t>Mask</t>
-  </si>
-  <si>
     <t>Inside</t>
   </si>
   <si>
     <t>http://www.shutterstock.com/video/clip-5092847-stock-footage-happy-attractive-young-woman-having-a-video-chat-as-seen-from-the-point-of-view-of-the-computer.html</t>
+  </si>
+  <si>
+    <t>http://www.flaticon.com/free-icon/visible-opened-eye-interface-option_58976</t>
+  </si>
+  <si>
+    <t>Eye</t>
+  </si>
+  <si>
+    <t>Hidden Eye</t>
+  </si>
+  <si>
+    <t>http://www.flaticon.com/free-icon/invisible_59394</t>
   </si>
 </sst>
 </file>
@@ -732,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,10 +1009,18 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1019,7 +1033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1051,10 +1065,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more missed visitor changes
pulling to check Rinkal's stuff
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\422Group4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>Door closed</t>
   </si>
@@ -412,6 +407,12 @@
   </si>
   <si>
     <t>http://www.flaticon.com/free-icon/invisible_59394</t>
+  </si>
+  <si>
+    <t>Missed Visitor 2</t>
+  </si>
+  <si>
+    <t>https://squareonemediauk.files.wordpress.com/2012/04/tom-7957.jpg</t>
   </si>
 </sst>
 </file>
@@ -730,7 +731,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -738,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,6 +1022,14 @@
       </c>
       <c r="B34" s="2" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>